<commit_message>
update xlsx b4 submission
</commit_message>
<xml_diff>
--- a/data/xlsx/QUEST-Bio.xlsx
+++ b/data/xlsx/QUEST-Bio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Denis/Desktop/QUEST/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Denis/Documents/Publis/Benchmarks-2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3DA6E5-D86C-5340-8E4C-F6B392B0E5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF62F602-175E-BD4F-A563-102C30C1D755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3740" yWindow="10180" windowWidth="30240" windowHeight="14560" xr2:uid="{E446C898-C1C5-6B4A-ADAC-A69F6B1D818F}"/>
   </bookViews>
@@ -1054,7 +1054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CEB361-C40C-E542-B9C0-9C732B51290B}">
   <dimension ref="A1:AH38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C21" sqref="C21:S33"/>
     </sheetView>
   </sheetViews>
@@ -2241,7 +2241,7 @@
         <v>32</v>
       </c>
       <c r="B21" s="8" t="str">
-        <f>B4</f>
+        <f t="shared" ref="B21:B33" si="2">B4</f>
         <v>A' (Val, pi-pi*)</v>
       </c>
       <c r="C21" s="9">
@@ -2289,7 +2289,7 @@
         <v>5.1769999999999996</v>
       </c>
       <c r="S21" s="2">
-        <f t="shared" ref="S21:S29" si="2">AVERAGE(Q21:R21)</f>
+        <f t="shared" ref="S21:S29" si="3">AVERAGE(Q21:R21)</f>
         <v>5.2059999999999995</v>
       </c>
       <c r="T21" s="14"/>
@@ -2311,7 +2311,7 @@
     <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="8" t="str">
-        <f>B5</f>
+        <f t="shared" si="2"/>
         <v>A' (Val, pi-pi*)</v>
       </c>
       <c r="C22" s="9">
@@ -2357,7 +2357,7 @@
         <v>5.2460000000000004</v>
       </c>
       <c r="S22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.2234999999999996</v>
       </c>
       <c r="T22" s="11"/>
@@ -2379,7 +2379,7 @@
     <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="8" t="str">
-        <f>B6</f>
+        <f t="shared" si="2"/>
         <v>A" (Val, n-pi*)</v>
       </c>
       <c r="C23" s="2">
@@ -2427,7 +2427,7 @@
         <v>5.5609999999999999</v>
       </c>
       <c r="S23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.35</v>
       </c>
       <c r="T23" s="9"/>
@@ -2449,7 +2449,7 @@
     <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="8" t="str">
-        <f>B7</f>
+        <f t="shared" si="2"/>
         <v>A" (Ryd, pi-R)</v>
       </c>
       <c r="C24" s="9">
@@ -2497,7 +2497,7 @@
         <v>5.5179999999999998</v>
       </c>
       <c r="S24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.5429999999999993</v>
       </c>
       <c r="T24" s="9"/>
@@ -2519,7 +2519,7 @@
     <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="8" t="str">
-        <f>B8</f>
+        <f t="shared" si="2"/>
         <v>A" (Val, n-pi*)</v>
       </c>
       <c r="C25" s="9">
@@ -2567,7 +2567,7 @@
         <v>6.101</v>
       </c>
       <c r="S25" s="2">
-        <f t="shared" ref="S25" si="3">AVERAGE(Q25:R25)</f>
+        <f t="shared" ref="S25" si="4">AVERAGE(Q25:R25)</f>
         <v>5.9165000000000001</v>
       </c>
       <c r="T25" s="9"/>
@@ -2589,7 +2589,7 @@
     <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="8" t="str">
-        <f>B9</f>
+        <f t="shared" si="2"/>
         <v>A" (Ryd, pi-R)</v>
       </c>
       <c r="C26" s="2">
@@ -2637,7 +2637,7 @@
         <v>5.87</v>
       </c>
       <c r="S26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.8819999999999997</v>
       </c>
       <c r="T26" s="9"/>
@@ -2659,7 +2659,7 @@
     <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="8" t="str">
-        <f>B10</f>
+        <f t="shared" si="2"/>
         <v>A' (Val, pi-pi*)</v>
       </c>
       <c r="C27" s="3"/>
@@ -2703,7 +2703,7 @@
         <v>6.4720000000000004</v>
       </c>
       <c r="S27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3920000000000003</v>
       </c>
       <c r="T27" s="9"/>
@@ -2725,7 +2725,7 @@
     <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="8" t="str">
-        <f>B11</f>
+        <f t="shared" si="2"/>
         <v>A' (Val, pi-pi*)</v>
       </c>
       <c r="C28" s="3"/>
@@ -2769,7 +2769,7 @@
         <v>6.4020000000000001</v>
       </c>
       <c r="S28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.4664999999999999</v>
       </c>
       <c r="T28" s="9"/>
@@ -2791,7 +2791,7 @@
     <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="8" t="str">
-        <f>B12</f>
+        <f t="shared" si="2"/>
         <v>A' (Ryd, n-R)</v>
       </c>
       <c r="C29" s="3"/>
@@ -2835,7 +2835,7 @@
         <v>7.0919999999999996</v>
       </c>
       <c r="S29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.6229999999999993</v>
       </c>
       <c r="T29" s="9"/>
@@ -2859,7 +2859,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="8" t="str">
-        <f>B13</f>
+        <f t="shared" si="2"/>
         <v>A' (Val, pi-pi*)</v>
       </c>
       <c r="C30" s="2">
@@ -2921,7 +2921,7 @@
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="8" t="str">
-        <f>B14</f>
+        <f t="shared" si="2"/>
         <v>A' (Val, pi-pi*)</v>
       </c>
       <c r="C31" s="9">
@@ -2983,7 +2983,7 @@
     <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="8" t="str">
-        <f>B15</f>
+        <f t="shared" si="2"/>
         <v>A" (Val, n-pi*)</v>
       </c>
       <c r="C32" s="2">
@@ -3045,7 +3045,7 @@
     <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="8" t="str">
-        <f>B16</f>
+        <f t="shared" si="2"/>
         <v>A" (Ryd, pi-R)</v>
       </c>
       <c r="C33" s="9">

</xml_diff>